<commit_message>
#2 #3 display and delete comment
</commit_message>
<xml_diff>
--- a/DATABASE DIAGRAM/Book1.xlsx
+++ b/DATABASE DIAGRAM/Book1.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20384"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Ulvy\PROJECTS\PHP-DB-G3\DATABASE DIAGRAM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sophiem.loem\Desktop\PHP-DB-G3\DATABASE DIAGRAM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{55F49236-CB0E-4C26-884A-7E8484F088B4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E83DB3-6966-4DC6-BBF5-3ADD211E83F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7070" xr2:uid="{4C4721BF-7EA5-42EC-977A-BFC4C1ADE578}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{4C4721BF-7EA5-42EC-977A-BFC4C1ADE578}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="36">
   <si>
     <t>USERS</t>
   </si>
@@ -237,15 +237,6 @@
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -257,6 +248,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2399,34 +2399,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{973E70E0-CDDA-4063-A0DF-04D9EE48DF4F}">
-  <dimension ref="B3:P20"/>
+  <dimension ref="B3:P19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="15.54296875" customWidth="1"/>
-    <col min="5" max="5" width="13.6328125" customWidth="1"/>
-    <col min="8" max="8" width="8.81640625" customWidth="1"/>
-    <col min="9" max="9" width="15.54296875" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" customWidth="1"/>
     <col min="10" max="10" width="15" customWidth="1"/>
-    <col min="15" max="15" width="17.26953125" customWidth="1"/>
-    <col min="16" max="16" width="15.26953125" customWidth="1"/>
+    <col min="15" max="15" width="17.28515625" customWidth="1"/>
+    <col min="16" max="16" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="C3" s="2" t="s">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="4"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="10"/>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
@@ -2436,11 +2436,11 @@
       <c r="E4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
         <v>3</v>
@@ -2448,13 +2448,13 @@
       <c r="E5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="7"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B6" s="9"/>
+      <c r="F5" s="4"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B6" s="6"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
         <v>4</v>
@@ -2462,11 +2462,11 @@
       <c r="E6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -2474,11 +2474,11 @@
       <c r="E7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
         <v>7</v>
@@ -2486,32 +2486,32 @@
       <c r="E8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C10" s="1"/>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="7" t="s">
         <v>32</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
         <v>33</v>
@@ -2520,25 +2520,25 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="D13" s="8"/>
-      <c r="N13" s="2" t="s">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D13" s="5"/>
+      <c r="N13" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="O13" s="3"/>
-      <c r="P13" s="4"/>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="H14" s="2" t="s">
+      <c r="O13" s="9"/>
+      <c r="P13" s="10"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="H14" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="I14" s="3"/>
-      <c r="J14" s="4"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="10"/>
       <c r="N14" s="1" t="s">
         <v>1</v>
       </c>
@@ -2549,12 +2549,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B15" s="9"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B15" s="6"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
       <c r="H15" s="1" t="s">
         <v>1</v>
       </c>
@@ -2574,14 +2574,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="H16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="N16" s="1"/>
       <c r="O16" s="1" t="s">
         <v>21</v>
@@ -2590,60 +2596,46 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="3:16" x14ac:dyDescent="0.35">
-      <c r="C17" s="5"/>
+    <row r="17" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C17" s="2"/>
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
-      <c r="H17" s="1" t="s">
+      <c r="H17" s="1"/>
+      <c r="I17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N17" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I17" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J17" s="1" t="s">
+      <c r="O17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="P17" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="N17" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="O17" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="P17" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="3:16" x14ac:dyDescent="0.35">
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
+    </row>
+    <row r="18" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="3:16" x14ac:dyDescent="0.35">
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J19" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="3:16" x14ac:dyDescent="0.35">
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
+    <row r="19" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2662,38 +2654,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3313CCA-97EF-4363-8483-1EB416F9879C}">
   <dimension ref="B3:S25"/>
   <sheetViews>
-    <sheetView zoomScale="89" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14:O18"/>
+    <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="15.54296875" customWidth="1"/>
-    <col min="5" max="5" width="13.6328125" customWidth="1"/>
-    <col min="8" max="8" width="8.81640625" customWidth="1"/>
-    <col min="9" max="9" width="15.54296875" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" customWidth="1"/>
     <col min="10" max="10" width="15" customWidth="1"/>
-    <col min="13" max="13" width="11.26953125" customWidth="1"/>
-    <col min="14" max="14" width="12.453125" customWidth="1"/>
-    <col min="15" max="15" width="11.6328125" customWidth="1"/>
+    <col min="13" max="13" width="11.28515625" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="C3" s="2" t="s">
+    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="C3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="4"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="10"/>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
-      <c r="M3" s="2" t="s">
+      <c r="M3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="N3" s="3"/>
-      <c r="O3" s="4"/>
-    </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="N3" s="9"/>
+      <c r="O3" s="10"/>
+    </row>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
@@ -2703,9 +2695,9 @@
       <c r="E4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
       <c r="M4" s="1" t="s">
         <v>1</v>
       </c>
@@ -2722,7 +2714,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
         <v>3</v>
@@ -2730,15 +2722,15 @@
       <c r="E5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="7"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
+      <c r="F5" s="4"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
       <c r="M5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>5</v>
@@ -2750,8 +2742,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B6" s="9">
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B6" s="6">
         <v>1</v>
       </c>
       <c r="C6" s="1"/>
@@ -2761,16 +2753,16 @@
       <c r="E6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="M6" s="1" t="s">
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="M6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="N6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="O6" s="1" t="s">
+      <c r="N6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="R6">
@@ -2780,7 +2772,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -2788,18 +2780,9 @@
       <c r="E7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="M7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="N7" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="O7" s="6" t="s">
-        <v>5</v>
-      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
       <c r="R7">
         <v>1</v>
       </c>
@@ -2807,7 +2790,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
         <v>7</v>
@@ -2815,9 +2798,9 @@
       <c r="E8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
       <c r="R8">
         <v>2</v>
       </c>
@@ -2825,28 +2808,28 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-    </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C10" s="1"/>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="7" t="s">
         <v>32</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
         <v>33</v>
@@ -2855,33 +2838,33 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="D13" s="8"/>
-    </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="C14" s="2" t="s">
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="D13" s="5"/>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="C14" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="4"/>
-      <c r="H14" s="2" t="s">
+      <c r="D14" s="9"/>
+      <c r="E14" s="10"/>
+      <c r="H14" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="I14" s="3"/>
-      <c r="J14" s="4"/>
-      <c r="M14" s="2" t="s">
+      <c r="I14" s="9"/>
+      <c r="J14" s="10"/>
+      <c r="M14" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="N14" s="3"/>
-      <c r="O14" s="4"/>
-    </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B15" s="9" t="s">
+      <c r="N14" s="9"/>
+      <c r="O14" s="10"/>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B15" s="6" t="s">
         <v>27</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -2912,7 +2895,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
         <v>9</v>
@@ -2939,7 +2922,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
         <v>2</v>
@@ -2964,7 +2947,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C18" s="1"/>
       <c r="D18" s="1" t="s">
         <v>21</v>
@@ -2979,17 +2962,17 @@
       <c r="J18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M18" s="6" t="s">
+      <c r="M18" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="N18" s="6" t="s">
+      <c r="N18" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O18" s="6" t="s">
+      <c r="O18" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C19" s="1"/>
       <c r="D19" s="1" t="s">
         <v>25</v>
@@ -3005,19 +2988,19 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:15" x14ac:dyDescent="0.25">
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
-    <row r="23" spans="3:15" x14ac:dyDescent="0.35">
-      <c r="C23" s="2" t="s">
+    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C23" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="4"/>
-    </row>
-    <row r="24" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="D23" s="9"/>
+      <c r="E23" s="10"/>
+    </row>
+    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C24" s="1" t="s">
         <v>10</v>
       </c>
@@ -3026,7 +3009,7 @@
       </c>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="3:15" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C25" s="1" t="s">
         <v>10</v>
       </c>

</xml_diff>